<commit_message>
toutes images en jpg
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,16 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solenne/Desktop/OC - Web développeur/P4_Lachouetteagence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E3865E-A071-9346-81FE-F6BEF2BF1D11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC341B2-D80A-B64D-9C82-D233B4507B67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page d'accueil" sheetId="1" r:id="rId1"/>
-    <sheet name="Page 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Page contact" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
     </ext>
@@ -26,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Catégorie</t>
   </si>
@@ -164,6 +173,18 @@
   </si>
   <si>
     <t xml:space="preserve">Dans le code HTML, définir la langue française pour le site internet </t>
+  </si>
+  <si>
+    <t>Certains liens n'ont pas de textes visibles</t>
+  </si>
+  <si>
+    <t>Les technologies d'assistance - comme le lecteur - ne pourront pas naviguer correctement sur ces liens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout d'un texte visible pour chaque lien </t>
+  </si>
+  <si>
+    <t>Recommandation Lighthouse</t>
   </si>
 </sst>
 </file>
@@ -488,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -650,7 +671,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="51">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -670,7 +691,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="51">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -710,7 +731,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -749,9 +770,24 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="E13" s="5" t="b">
-        <v>0</v>
+    <row r="13" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>